<commit_message>
Updated templates to highlight user added fields and correct a couple of small bugs
</commit_message>
<xml_diff>
--- a/resources/templates/NOMADS_Library_Worksheet.xlsx
+++ b/resources/templates/NOMADS_Library_Worksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\templates\experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C422647-B289-4D3D-B5EF-B1A16D052529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0156D473-4E86-459A-9B24-DD3B87489898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="368">
   <si>
     <t>ng</t>
   </si>
@@ -1142,19 +1142,7 @@
     <t>User</t>
   </si>
   <si>
-    <t>Brenda Mambwe</t>
-  </si>
-  <si>
-    <t>Mulenga Mwenda</t>
-  </si>
-  <si>
     <t>Initials</t>
-  </si>
-  <si>
-    <t>BM</t>
-  </si>
-  <si>
-    <t>MM</t>
   </si>
   <si>
     <t>Exp ID:</t>
@@ -1358,9 +1346,6 @@
     <t>reference</t>
   </si>
   <si>
-    <t>contains look-up tables, assumptions etc</t>
-  </si>
-  <si>
     <t>exp_metadata</t>
   </si>
   <si>
@@ -1422,18 +1407,6 @@
   </si>
   <si>
     <t>Batch:</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>TES2022</t>
-  </si>
-  <si>
-    <t>GenE8</t>
-  </si>
-  <si>
-    <t>TES2023</t>
   </si>
   <si>
     <t>(e.g. A, B, C etc)</t>
@@ -1467,6 +1440,46 @@
       </rPr>
       <t xml:space="preserve"> script in this repository:</t>
     </r>
+  </si>
+  <si>
+    <t>User-defined</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Fiona Waiting</t>
+  </si>
+  <si>
+    <t>FW</t>
+  </si>
+  <si>
+    <t>Terence Broad</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>contains look-up tables, assumptions etc. Edit the entries in green according to your needs</t>
+  </si>
+  <si>
+    <t>NB. The entries above are used for dropdown options in other tabs. To add additional entries and maintain the dropdowns, do the following:</t>
+  </si>
+  <si>
+    <t>4. Enter the new details into the new row</t>
+  </si>
+  <si>
+    <t>3. Select 'Shift cells down'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Right click on the highlighted cells and select 'insert'
+</t>
+  </si>
+  <si>
+    <t>1. Select a complete entry i.e. for names you would highlight two cells e.g. G5 and H5</t>
   </si>
 </sst>
 </file>
@@ -1609,7 +1622,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1679,6 +1692,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1828,7 +1847,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2002,22 +2021,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2026,13 +2101,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2046,9 +2124,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -2071,68 +2146,17 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3042,7 +3066,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:H10"/>
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3051,140 +3075,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
-        <v>282</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
+      <c r="A1" s="100" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="91" t="s">
         <v>257</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="80" t="s">
+      <c r="B2" s="92"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="85" t="s">
         <v>266</v>
       </c>
-      <c r="H2" s="80"/>
-      <c r="J2" s="78" t="s">
+      <c r="H2" s="85"/>
+      <c r="J2" s="99" t="s">
         <v>265</v>
       </c>
-      <c r="K2" s="78"/>
+      <c r="K2" s="99"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
       <c r="G3" t="s">
-        <v>275</v>
-      </c>
-      <c r="J3" s="76" t="s">
+        <v>271</v>
+      </c>
+      <c r="J3" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="76"/>
+      <c r="K3" s="97"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
-        <v>281</v>
-      </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="A4" s="91" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="92"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
       <c r="G4" s="50" t="s">
-        <v>316</v>
-      </c>
-      <c r="J4" s="77" t="s">
+        <v>312</v>
+      </c>
+      <c r="J4" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="77"/>
+      <c r="K4" s="98"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
-        <v>274</v>
-      </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="85" t="str">
-        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",_xlfn.CONCAT("SL",VLOOKUP(C3,reference!E7:F8,2,FALSE),C4))</f>
-        <v/>
-      </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="A5" s="101" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="102"/>
+      <c r="C5" s="105" t="str">
+        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",_xlfn.CONCAT("SL",VLOOKUP(C3,reference!G3:H5,2,FALSE),C4))</f>
+        <v/>
+      </c>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="30" t="s">
-        <v>293</v>
-      </c>
-      <c r="J5" s="87" t="s">
-        <v>361</v>
-      </c>
-      <c r="K5" s="87"/>
+        <v>289</v>
+      </c>
+      <c r="J5" s="107" t="s">
+        <v>352</v>
+      </c>
+      <c r="K5" s="107"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="101" t="s">
         <v>258</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="66" t="str">
+      <c r="B6" s="102"/>
+      <c r="C6" s="108" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",_xlfn.CONCAT(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
       <c r="G6" s="47"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
-        <v>354</v>
-      </c>
-      <c r="B7" s="104"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
+      <c r="A7" s="69" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" s="69"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104" t="s">
-        <v>355</v>
-      </c>
-      <c r="B8" s="104"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
+      <c r="A8" s="69" t="s">
+        <v>350</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
       <c r="G8" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="103" t="s">
-        <v>347</v>
-      </c>
-      <c r="B9" s="103"/>
+      <c r="A9" s="68" t="s">
+        <v>342</v>
+      </c>
+      <c r="B9" s="68"/>
       <c r="C9" s="90" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",_xlfn.CONCAT(C7,"_Batch",C8))</f>
         <v/>
@@ -3193,62 +3217,62 @@
       <c r="E9" s="90"/>
       <c r="F9" s="90"/>
       <c r="G9" s="30" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
-        <v>353</v>
-      </c>
-      <c r="B10" s="103"/>
-      <c r="C10" s="105" t="str">
+      <c r="A10" s="68" t="s">
+        <v>348</v>
+      </c>
+      <c r="B10" s="68"/>
+      <c r="C10" s="70" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",_xlfn.CONCAT(C6,"_",exp_summary,".xlsm"))</f>
         <v/>
       </c>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="91" t="s">
         <v>259</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
       <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="71" t="s">
-        <v>343</v>
-      </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="91"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="91"/>
+      <c r="A12" s="91" t="s">
+        <v>338</v>
+      </c>
+      <c r="B12" s="92"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="93"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="57"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="91"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="91"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="93"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
@@ -3261,18 +3285,18 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="14"/>
       <c r="D15" s="10"/>
       <c r="G15" s="15"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="74" t="s">
-        <v>288</v>
-      </c>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
+      <c r="I15" s="110" t="s">
+        <v>284</v>
+      </c>
+      <c r="J15" s="110"/>
+      <c r="K15" s="110"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="str">
@@ -3304,121 +3328,121 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:11" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="95" t="s">
+      <c r="A18" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="95"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="69" t="s">
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69" t="str">
+      <c r="E18" s="77"/>
+      <c r="F18" s="77" t="str">
         <f>_xlfn.CONCAT("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="69"/>
-      <c r="I18" s="70" t="s">
+      <c r="G18" s="77"/>
+      <c r="I18" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="J18" s="70"/>
+      <c r="J18" s="86"/>
       <c r="K18" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="97" t="s">
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="97"/>
-      <c r="F19" s="73" t="s">
+      <c r="E19" s="76"/>
+      <c r="F19" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="73"/>
-      <c r="I19" s="67">
+      <c r="G19" s="109"/>
+      <c r="I19" s="72">
         <v>20</v>
       </c>
-      <c r="J19" s="67"/>
+      <c r="J19" s="72"/>
       <c r="K19" s="15">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="97" t="str">
+      <c r="B20" s="84"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="76" t="str">
         <f>_xlfn.CONCAT(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E20" s="97"/>
-      <c r="F20" s="73" t="s">
+      <c r="E20" s="76"/>
+      <c r="F20" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="G20" s="73"/>
-      <c r="I20" s="67">
+      <c r="G20" s="109"/>
+      <c r="I20" s="72">
         <v>65</v>
       </c>
-      <c r="J20" s="67"/>
+      <c r="J20" s="72"/>
       <c r="K20" s="15">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="68" t="s">
+      <c r="A21" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="68"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="96">
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="95">
         <v>1.4</v>
       </c>
-      <c r="E21" s="96"/>
-      <c r="F21" s="73">
+      <c r="E21" s="95"/>
+      <c r="F21" s="109">
         <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="73"/>
-      <c r="I21" s="67">
+      <c r="G21" s="109"/>
+      <c r="I21" s="72">
         <v>4</v>
       </c>
-      <c r="J21" s="67"/>
+      <c r="J21" s="72"/>
       <c r="K21" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="96">
+      <c r="B22" s="84"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="95">
         <v>0.6</v>
       </c>
-      <c r="E22" s="96"/>
-      <c r="F22" s="73">
+      <c r="E22" s="95"/>
+      <c r="F22" s="109">
         <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="73"/>
+      <c r="G22" s="109"/>
       <c r="H22" s="10"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="D23" s="75">
+      <c r="D23" s="111">
         <f>SUM(D21:D22)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E23" s="75"/>
+      <c r="E23" s="111"/>
       <c r="F23" s="20" t="str">
         <f>_xlfn.CONCAT("Add ",SUM(D21:D22)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
@@ -3454,104 +3478,104 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:11" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="95" t="s">
+      <c r="A26" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="95"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="69" t="s">
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69" t="str">
+      <c r="E26" s="77"/>
+      <c r="F26" s="77" t="str">
         <f>_xlfn.CONCAT("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G26" s="69"/>
+      <c r="G26" s="77"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="70" t="s">
+      <c r="I26" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="70"/>
+      <c r="J26" s="86"/>
       <c r="K26" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="97">
+      <c r="B27" s="84"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="76">
         <v>0.5</v>
       </c>
-      <c r="E27" s="97"/>
-      <c r="F27" s="73" t="s">
+      <c r="E27" s="76"/>
+      <c r="F27" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="73"/>
-      <c r="I27" s="67">
+      <c r="G27" s="109"/>
+      <c r="I27" s="72">
         <v>20</v>
       </c>
-      <c r="J27" s="67"/>
+      <c r="J27" s="72"/>
       <c r="K27" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="97">
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="76">
         <v>6</v>
       </c>
-      <c r="E28" s="97"/>
-      <c r="F28" s="73">
+      <c r="E28" s="76"/>
+      <c r="F28" s="109">
         <f>SUM(D28*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="73"/>
-      <c r="I28" s="67">
+      <c r="G28" s="109"/>
+      <c r="I28" s="72">
         <v>65</v>
       </c>
-      <c r="J28" s="67"/>
+      <c r="J28" s="72"/>
       <c r="K28" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="97">
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="76">
         <v>0.2</v>
       </c>
-      <c r="E29" s="97"/>
-      <c r="F29" s="73">
+      <c r="E29" s="76"/>
+      <c r="F29" s="109">
         <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="73"/>
-      <c r="I29" s="67">
+      <c r="G29" s="109"/>
+      <c r="I29" s="72">
         <v>8</v>
       </c>
-      <c r="J29" s="67"/>
+      <c r="J29" s="72"/>
       <c r="K29" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="D30" s="106">
+      <c r="D30" s="75">
         <f>SUM(D27:D29)+D23</f>
         <v>18.7</v>
       </c>
-      <c r="E30" s="106"/>
+      <c r="E30" s="75"/>
       <c r="F30" s="20" t="str">
         <f>_xlfn.CONCAT("Add ",SUM(D28:D29)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
@@ -3561,7 +3585,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="14"/>
@@ -3579,20 +3603,20 @@
       <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80" t="s">
+      <c r="A34" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="80"/>
-      <c r="C34" s="80"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="80"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="80"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="85"/>
+      <c r="J34" s="85"/>
+      <c r="K34" s="85"/>
+      <c r="L34" s="85"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
@@ -3615,10 +3639,10 @@
       <c r="C36" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="99" t="s">
+      <c r="D36" s="87" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="94"/>
+      <c r="E36" s="88"/>
     </row>
     <row r="37" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26">
@@ -3627,11 +3651,11 @@
       </c>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
-      <c r="D37" s="107">
+      <c r="D37" s="80">
         <f>SUM(B37*C37)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="107"/>
+      <c r="E37" s="80"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F38"/>
@@ -3640,7 +3664,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -3662,126 +3686,126 @@
       <c r="H40"/>
     </row>
     <row r="41" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="93" t="s">
+      <c r="B41" s="86"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="93"/>
+      <c r="E41" s="94"/>
       <c r="F41" s="10"/>
       <c r="H41"/>
-      <c r="I41" s="70" t="s">
+      <c r="I41" s="86" t="s">
         <v>106</v>
       </c>
-      <c r="J41" s="70"/>
+      <c r="J41" s="86"/>
       <c r="K41" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="68" t="s">
+      <c r="A42" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="92">
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="74">
         <f>IF(B37="",adaptlig_maxvol,IF(SUM(adaptlig_targetmass/D37)&gt;adaptlig_maxvol,adaptlig_maxvol,SUM(adaptlig_targetmass/D37)))</f>
         <v>65</v>
       </c>
-      <c r="E42" s="92"/>
+      <c r="E42" s="74"/>
       <c r="F42" s="12"/>
       <c r="G42" s="10"/>
       <c r="H42"/>
-      <c r="I42" s="67" t="s">
+      <c r="I42" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="J42" s="67"/>
+      <c r="J42" s="72"/>
       <c r="K42" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="68" t="s">
+      <c r="A43" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="92">
+      <c r="B43" s="84"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="74">
         <f>IFERROR(SUM(adaptlig_maxvol-D42),"")</f>
         <v>0</v>
       </c>
-      <c r="E43" s="92"/>
+      <c r="E43" s="74"/>
       <c r="F43" s="15"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="84" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="89">
+      <c r="B44" s="84"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="79">
         <v>5</v>
       </c>
-      <c r="E44" s="89"/>
+      <c r="E44" s="79"/>
       <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="68" t="s">
+      <c r="A45" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="89">
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="79">
         <v>20</v>
       </c>
-      <c r="E45" s="89"/>
+      <c r="E45" s="79"/>
       <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="68" t="s">
+      <c r="A46" s="84" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="68"/>
-      <c r="C46" s="68"/>
-      <c r="D46" s="89">
+      <c r="B46" s="84"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="79">
         <v>10</v>
       </c>
-      <c r="E46" s="89"/>
+      <c r="E46" s="79"/>
       <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="C47" s="10"/>
-      <c r="D47" s="102">
+      <c r="D47" s="89">
         <f>SUM(D42:D46)</f>
         <v>100</v>
       </c>
-      <c r="E47" s="102"/>
+      <c r="E47" s="89"/>
       <c r="F47" s="10"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="80" t="s">
+      <c r="A50" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="80"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="80"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="80"/>
-      <c r="J50" s="80"/>
-      <c r="K50" s="80"/>
-      <c r="L50" s="80"/>
+      <c r="B50" s="85"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="85"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="85"/>
+      <c r="K50" s="85"/>
+      <c r="L50" s="85"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
@@ -3795,42 +3819,42 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="B52" s="98"/>
-      <c r="C52" s="95" t="s">
+      <c r="B52" s="81"/>
+      <c r="C52" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="95"/>
-      <c r="E52" s="95" t="s">
+      <c r="D52" s="78"/>
+      <c r="E52" s="78" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="95"/>
-      <c r="G52" s="98" t="s">
+      <c r="F52" s="78"/>
+      <c r="G52" s="81" t="s">
         <v>132</v>
       </c>
-      <c r="H52" s="95"/>
+      <c r="H52" s="78"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="108">
+      <c r="A53" s="82">
         <f>SUM(D47*0.5)</f>
         <v>50</v>
       </c>
-      <c r="B53" s="108"/>
-      <c r="C53" s="101"/>
-      <c r="D53" s="101"/>
-      <c r="E53" s="101"/>
-      <c r="F53" s="101"/>
-      <c r="G53" s="68">
+      <c r="B53" s="82"/>
+      <c r="C53" s="83"/>
+      <c r="D53" s="83"/>
+      <c r="E53" s="83"/>
+      <c r="F53" s="83"/>
+      <c r="G53" s="84">
         <f>SUM(C53*E53)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="68"/>
+      <c r="H53" s="84"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -3844,61 +3868,61 @@
       <c r="C56" s="10"/>
     </row>
     <row r="57" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="70" t="s">
+      <c r="A57" s="86" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="70"/>
-      <c r="C57" s="70"/>
-      <c r="D57" s="93" t="s">
+      <c r="B57" s="86"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="E57" s="93"/>
+      <c r="E57" s="94"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="94" t="s">
+      <c r="A58" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="B58" s="94"/>
-      <c r="C58" s="94"/>
-      <c r="D58" s="92">
+      <c r="B58" s="88"/>
+      <c r="C58" s="88"/>
+      <c r="D58" s="74">
         <f>IF(C53="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G53)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G53)))</f>
         <v>12</v>
       </c>
-      <c r="E58" s="92"/>
+      <c r="E58" s="74"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="94" t="s">
+      <c r="A59" s="88" t="s">
         <v>135</v>
       </c>
-      <c r="B59" s="94"/>
-      <c r="C59" s="94"/>
-      <c r="D59" s="92" t="str">
+      <c r="B59" s="88"/>
+      <c r="C59" s="88"/>
+      <c r="D59" s="74" t="str">
         <f>IFERROR((IF(SUM(12-D58)=0,"-",SUM(12-D58))),"")</f>
         <v>-</v>
       </c>
-      <c r="E59" s="92"/>
+      <c r="E59" s="74"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="68" t="s">
+      <c r="A60" s="84" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="68"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="100">
+      <c r="B60" s="84"/>
+      <c r="C60" s="84"/>
+      <c r="D60" s="73">
         <v>37.5</v>
       </c>
-      <c r="E60" s="100"/>
+      <c r="E60" s="73"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="68" t="s">
+      <c r="A61" s="84" t="s">
         <v>143</v>
       </c>
-      <c r="B61" s="68"/>
-      <c r="C61" s="68"/>
-      <c r="D61" s="100">
+      <c r="B61" s="84"/>
+      <c r="C61" s="84"/>
+      <c r="D61" s="73">
         <v>25.5</v>
       </c>
-      <c r="E61" s="100"/>
+      <c r="E61" s="73"/>
       <c r="F61" s="12" t="s">
         <v>142</v>
       </c>
@@ -3914,82 +3938,175 @@
       <c r="C63" s="21"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="71" t="s">
-        <v>276</v>
-      </c>
-      <c r="B64" s="72"/>
-      <c r="C64" s="88" t="s">
-        <v>277</v>
-      </c>
-      <c r="D64" s="68"/>
+      <c r="A64" s="91" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" s="92"/>
+      <c r="C64" s="96" t="s">
+        <v>273</v>
+      </c>
+      <c r="D64" s="84"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="72" t="s">
+      <c r="A65" s="92" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="68"/>
-      <c r="D65" s="68"/>
+      <c r="B65" s="92"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="72" t="s">
+      <c r="A66" s="92" t="s">
         <v>261</v>
       </c>
-      <c r="B66" s="72"/>
-      <c r="C66" s="68"/>
-      <c r="D66" s="68"/>
+      <c r="B66" s="92"/>
+      <c r="C66" s="84"/>
+      <c r="D66" s="84"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="72" t="s">
-        <v>306</v>
-      </c>
-      <c r="B67" s="72"/>
-      <c r="C67" s="89" t="str">
+      <c r="A67" s="92" t="s">
+        <v>302</v>
+      </c>
+      <c r="B67" s="92"/>
+      <c r="C67" s="79" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D67" s="89"/>
+      <c r="D67" s="79"/>
       <c r="E67" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="72" t="s">
+      <c r="A68" s="92" t="s">
         <v>262</v>
       </c>
-      <c r="B68" s="72"/>
-      <c r="C68" s="68" t="s">
+      <c r="B68" s="92"/>
+      <c r="C68" s="84" t="s">
         <v>263</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="84"/>
       <c r="E68" s="11" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="72" t="s">
+      <c r="A69" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="B69" s="72"/>
-      <c r="C69" s="68"/>
-      <c r="D69" s="68"/>
+      <c r="B69" s="92"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="84"/>
       <c r="E69" s="11" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="72" t="s">
+      <c r="A70" s="92" t="s">
         <v>153</v>
       </c>
-      <c r="B70" s="72"/>
-      <c r="C70" s="68"/>
-      <c r="D70" s="68"/>
+      <c r="B70" s="92"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="84"/>
       <c r="E70" s="11" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="117">
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4014,99 +4131,6 @@
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A34:L34"/>
     <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C4 C7:C8 C11:C12 B37:C37 C53:E53 C64:C66 C68:C70">
     <cfRule type="expression" dxfId="8" priority="5">
@@ -4171,17 +4195,17 @@
           </x14:formula1>
           <xm:sqref>C66</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." xr:uid="{8C7E2C1B-80DC-4BB6-92F9-B434AEC4D204}">
+          <x14:formula1>
+            <xm:f>reference!$E$11:$E$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7:F7</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E7C7338-D4B5-4229-8F49-1913883BAA1F}">
           <x14:formula1>
-            <xm:f>reference!$E$7:$E$8</xm:f>
+            <xm:f>reference!$G$3:$G$5</xm:f>
           </x14:formula1>
           <xm:sqref>C3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." xr:uid="{8C7E2C1B-80DC-4BB6-92F9-B434AEC4D204}">
-          <x14:formula1>
-            <xm:f>reference!$E$15:$E$18</xm:f>
-          </x14:formula1>
-          <xm:sqref>C7:F7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4211,25 +4235,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="112" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="110"/>
+      <c r="D1" s="113"/>
       <c r="E1" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="111" t="s">
+      <c r="F1" s="114" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="114" t="s">
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="117" t="s">
         <v>117</v>
       </c>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="48.75" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
@@ -4245,31 +4269,31 @@
         <v>113</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H2" s="38" t="s">
         <v>256</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>255</v>
       </c>
       <c r="K2" s="39" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="L2" s="39" t="s">
         <v>169</v>
       </c>
       <c r="M2" s="39" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7565,7 +7589,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7581,77 +7605,77 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -7665,20 +7689,20 @@
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.25" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="6" max="6" width="5.125" customWidth="1"/>
+    <col min="7" max="7" width="19.75" customWidth="1"/>
+    <col min="8" max="8" width="8.75" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
     <col min="10" max="10" width="22.625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.875" customWidth="1"/>
@@ -7693,7 +7717,9 @@
       <c r="E1" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="7" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
@@ -7704,10 +7730,16 @@
       <c r="E2" s="49" t="s">
         <v>138</v>
       </c>
+      <c r="G2" s="65" t="s">
+        <v>268</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -7718,10 +7750,16 @@
       <c r="E3" t="s">
         <v>139</v>
       </c>
+      <c r="G3" s="66" t="s">
+        <v>356</v>
+      </c>
+      <c r="H3" s="66" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -7733,10 +7771,16 @@
       <c r="E4" t="s">
         <v>140</v>
       </c>
+      <c r="G4" s="66" t="s">
+        <v>358</v>
+      </c>
+      <c r="H4" s="66" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B5">
         <v>800</v>
@@ -7745,10 +7789,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="8"/>
+      <c r="G5" s="66" t="s">
+        <v>360</v>
+      </c>
+      <c r="H5" s="66" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B6">
         <v>65</v>
@@ -7757,15 +7807,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>268</v>
-      </c>
-      <c r="F6" s="49" t="s">
-        <v>271</v>
+        <v>138</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -7774,15 +7824,15 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>269</v>
-      </c>
-      <c r="F7" t="s">
-        <v>272</v>
+        <v>139</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -7791,75 +7841,61 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>270</v>
-      </c>
-      <c r="F8" t="s">
-        <v>273</v>
+        <v>140</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G9" s="67" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
-      <c r="E10" s="49" t="s">
-        <v>138</v>
+      <c r="G10" s="67" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B11" t="s">
-        <v>315</v>
-      </c>
-      <c r="E11" t="s">
-        <v>139</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B12">
         <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>140</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="14" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="49" t="s">
-        <v>356</v>
-      </c>
-    </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="2"/>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="1048576" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G1048576" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7889,73 +7925,73 @@
   <sheetData>
     <row r="1" spans="1:23" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -8084,28 +8120,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="G1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More error catching / formatting
</commit_message>
<xml_diff>
--- a/resources/templates/NOMADS_Library_Worksheet.xlsx
+++ b/resources/templates/NOMADS_Library_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitrepos\warehouse\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0156D473-4E86-459A-9B24-DD3B87489898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9281396B-F627-4ECA-ACC6-725C77E0D5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{202E2ACC-7D07-5944-B6D6-A1D8A2363375}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="372">
   <si>
     <t>ng</t>
   </si>
@@ -1480,6 +1480,18 @@
   </si>
   <si>
     <t>1. Select a complete entry i.e. for names you would highlight two cells e.g. G5 and H5</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>CoRE</t>
+  </si>
+  <si>
+    <t>ProACT</t>
+  </si>
+  <si>
+    <t>MIS2024</t>
   </si>
 </sst>
 </file>
@@ -2026,73 +2038,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2101,16 +2062,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2124,6 +2082,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -2146,17 +2107,68 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3066,7 +3078,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:F3"/>
+      <selection activeCell="C7" sqref="C7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3075,204 +3087,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="82" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="74" t="s">
         <v>257</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="85" t="s">
+      <c r="B2" s="75"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="83" t="s">
         <v>266</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="J2" s="99" t="s">
+      <c r="H2" s="83"/>
+      <c r="J2" s="81" t="s">
         <v>265</v>
       </c>
-      <c r="K2" s="99"/>
+      <c r="K2" s="81"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="74" t="s">
         <v>267</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
       <c r="G3" t="s">
         <v>271</v>
       </c>
-      <c r="J3" s="97" t="s">
+      <c r="J3" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="97"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="74" t="s">
         <v>277</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
       <c r="G4" s="50" t="s">
         <v>312</v>
       </c>
-      <c r="J4" s="98" t="s">
+      <c r="J4" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="K4" s="98"/>
+      <c r="K4" s="80"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="84" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="105" t="str">
+      <c r="B5" s="85"/>
+      <c r="C5" s="88" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",_xlfn.CONCAT("SL",VLOOKUP(C3,reference!G3:H5,2,FALSE),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
       <c r="G5" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="J5" s="107" t="s">
+      <c r="J5" s="90" t="s">
         <v>352</v>
       </c>
-      <c r="K5" s="107"/>
+      <c r="K5" s="90"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="84" t="s">
         <v>258</v>
       </c>
-      <c r="B6" s="102"/>
-      <c r="C6" s="108" t="str">
+      <c r="B6" s="85"/>
+      <c r="C6" s="69" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",_xlfn.CONCAT(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="47"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="107" t="s">
         <v>349</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
       <c r="G7" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="107" t="s">
         <v>350</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
       <c r="G8" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="106" t="s">
         <v>342</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="90" t="str">
+      <c r="B9" s="106"/>
+      <c r="C9" s="93" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",_xlfn.CONCAT(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
       <c r="G9" s="30" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="106" t="s">
         <v>348</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="70" t="str">
-        <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",_xlfn.CONCAT(C6,"_",exp_summary,".xlsm"))</f>
-        <v/>
-      </c>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="108" t="str">
+        <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",_xlfn.CONCAT(C6,"_",exp_summary,".xlsa"))</f>
+        <v/>
+      </c>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="108"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="74" t="s">
         <v>259</v>
       </c>
-      <c r="B11" s="92"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
       <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="93"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="94"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="57"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="94"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
@@ -3292,11 +3304,11 @@
       <c r="D15" s="10"/>
       <c r="G15" s="15"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="110" t="s">
+      <c r="I15" s="77" t="s">
         <v>284</v>
       </c>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="str">
@@ -3328,121 +3340,121 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:11" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="77" t="s">
+      <c r="B18" s="98"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77" t="str">
+      <c r="E18" s="72"/>
+      <c r="F18" s="72" t="str">
         <f>_xlfn.CONCAT("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="77"/>
-      <c r="I18" s="86" t="s">
+      <c r="G18" s="72"/>
+      <c r="I18" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="J18" s="86"/>
+      <c r="J18" s="73"/>
       <c r="K18" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="76" t="s">
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="100" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="76"/>
-      <c r="F19" s="109" t="s">
+      <c r="E19" s="100"/>
+      <c r="F19" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="109"/>
-      <c r="I19" s="72">
+      <c r="G19" s="76"/>
+      <c r="I19" s="70">
         <v>20</v>
       </c>
-      <c r="J19" s="72"/>
+      <c r="J19" s="70"/>
       <c r="K19" s="15">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="84" t="s">
+      <c r="A20" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="84"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="76" t="str">
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="100" t="str">
         <f>_xlfn.CONCAT(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E20" s="76"/>
-      <c r="F20" s="109" t="s">
+      <c r="E20" s="100"/>
+      <c r="F20" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="G20" s="109"/>
-      <c r="I20" s="72">
+      <c r="G20" s="76"/>
+      <c r="I20" s="70">
         <v>65</v>
       </c>
-      <c r="J20" s="72"/>
+      <c r="J20" s="70"/>
       <c r="K20" s="15">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="84" t="s">
+      <c r="A21" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="95">
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="99">
         <v>1.4</v>
       </c>
-      <c r="E21" s="95"/>
-      <c r="F21" s="109">
+      <c r="E21" s="99"/>
+      <c r="F21" s="76">
         <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="109"/>
-      <c r="I21" s="72">
+      <c r="G21" s="76"/>
+      <c r="I21" s="70">
         <v>4</v>
       </c>
-      <c r="J21" s="72"/>
+      <c r="J21" s="70"/>
       <c r="K21" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="84" t="s">
+      <c r="A22" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="95">
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="99">
         <v>0.6</v>
       </c>
-      <c r="E22" s="95"/>
-      <c r="F22" s="109">
+      <c r="E22" s="99"/>
+      <c r="F22" s="76">
         <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="109"/>
+      <c r="G22" s="76"/>
       <c r="H22" s="10"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="D23" s="111">
+      <c r="D23" s="78">
         <f>SUM(D21:D22)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E23" s="111"/>
+      <c r="E23" s="78"/>
       <c r="F23" s="20" t="str">
         <f>_xlfn.CONCAT("Add ",SUM(D21:D22)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
@@ -3478,104 +3490,104 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:11" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="77" t="s">
+      <c r="B26" s="98"/>
+      <c r="C26" s="98"/>
+      <c r="D26" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77" t="str">
+      <c r="E26" s="72"/>
+      <c r="F26" s="72" t="str">
         <f>_xlfn.CONCAT("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G26" s="77"/>
+      <c r="G26" s="72"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="86" t="s">
+      <c r="I26" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="86"/>
+      <c r="J26" s="73"/>
       <c r="K26" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="84" t="s">
+      <c r="A27" s="71" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="76">
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="100">
         <v>0.5</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="109" t="s">
+      <c r="E27" s="100"/>
+      <c r="F27" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="109"/>
-      <c r="I27" s="72">
+      <c r="G27" s="76"/>
+      <c r="I27" s="70">
         <v>20</v>
       </c>
-      <c r="J27" s="72"/>
+      <c r="J27" s="70"/>
       <c r="K27" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="84" t="s">
+      <c r="A28" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="76">
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="100">
         <v>6</v>
       </c>
-      <c r="E28" s="76"/>
-      <c r="F28" s="109">
+      <c r="E28" s="100"/>
+      <c r="F28" s="76">
         <f>SUM(D28*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="109"/>
-      <c r="I28" s="72">
+      <c r="G28" s="76"/>
+      <c r="I28" s="70">
         <v>65</v>
       </c>
-      <c r="J28" s="72"/>
+      <c r="J28" s="70"/>
       <c r="K28" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="84" t="s">
+      <c r="A29" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="76">
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="100">
         <v>0.2</v>
       </c>
-      <c r="E29" s="76"/>
-      <c r="F29" s="109">
+      <c r="E29" s="100"/>
+      <c r="F29" s="76">
         <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="109"/>
-      <c r="I29" s="72">
+      <c r="G29" s="76"/>
+      <c r="I29" s="70">
         <v>8</v>
       </c>
-      <c r="J29" s="72"/>
+      <c r="J29" s="70"/>
       <c r="K29" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="D30" s="75">
+      <c r="D30" s="109">
         <f>SUM(D27:D29)+D23</f>
         <v>18.7</v>
       </c>
-      <c r="E30" s="75"/>
+      <c r="E30" s="109"/>
       <c r="F30" s="20" t="str">
         <f>_xlfn.CONCAT("Add ",SUM(D28:D29)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
@@ -3603,20 +3615,20 @@
       <c r="G33" s="19"/>
     </row>
     <row r="34" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="83" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="85"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="85"/>
-      <c r="J34" s="85"/>
-      <c r="K34" s="85"/>
-      <c r="L34" s="85"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
+      <c r="L34" s="83"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
@@ -3639,10 +3651,10 @@
       <c r="C36" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="87" t="s">
+      <c r="D36" s="102" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="88"/>
+      <c r="E36" s="97"/>
     </row>
     <row r="37" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26">
@@ -3651,11 +3663,11 @@
       </c>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
-      <c r="D37" s="80">
+      <c r="D37" s="110">
         <f>SUM(B37*C37)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="80"/>
+      <c r="E37" s="110"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F38"/>
@@ -3686,104 +3698,104 @@
       <c r="H40"/>
     </row>
     <row r="41" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="86" t="s">
+      <c r="A41" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="94" t="s">
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="94"/>
+      <c r="E41" s="96"/>
       <c r="F41" s="10"/>
       <c r="H41"/>
-      <c r="I41" s="86" t="s">
+      <c r="I41" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="J41" s="86"/>
+      <c r="J41" s="73"/>
       <c r="K41" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="84" t="s">
+      <c r="A42" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="84"/>
-      <c r="C42" s="84"/>
-      <c r="D42" s="74">
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="95">
         <f>IF(B37="",adaptlig_maxvol,IF(SUM(adaptlig_targetmass/D37)&gt;adaptlig_maxvol,adaptlig_maxvol,SUM(adaptlig_targetmass/D37)))</f>
         <v>65</v>
       </c>
-      <c r="E42" s="74"/>
+      <c r="E42" s="95"/>
       <c r="F42" s="12"/>
       <c r="G42" s="10"/>
       <c r="H42"/>
-      <c r="I42" s="72" t="s">
+      <c r="I42" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="J42" s="72"/>
+      <c r="J42" s="70"/>
       <c r="K42" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="84" t="s">
+      <c r="A43" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="B43" s="84"/>
-      <c r="C43" s="84"/>
-      <c r="D43" s="74">
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="95">
         <f>IFERROR(SUM(adaptlig_maxvol-D42),"")</f>
         <v>0</v>
       </c>
-      <c r="E43" s="74"/>
+      <c r="E43" s="95"/>
       <c r="F43" s="15"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="84" t="s">
+      <c r="A44" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="84"/>
-      <c r="C44" s="84"/>
-      <c r="D44" s="79">
+      <c r="B44" s="71"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="92">
         <v>5</v>
       </c>
-      <c r="E44" s="79"/>
+      <c r="E44" s="92"/>
       <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="84" t="s">
+      <c r="A45" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="79">
+      <c r="B45" s="71"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="92">
         <v>20</v>
       </c>
-      <c r="E45" s="79"/>
+      <c r="E45" s="92"/>
       <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="84" t="s">
+      <c r="A46" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="84"/>
-      <c r="C46" s="84"/>
-      <c r="D46" s="79">
+      <c r="B46" s="71"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="92">
         <v>10</v>
       </c>
-      <c r="E46" s="79"/>
+      <c r="E46" s="92"/>
       <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="C47" s="10"/>
-      <c r="D47" s="89">
+      <c r="D47" s="105">
         <f>SUM(D42:D46)</f>
         <v>100</v>
       </c>
-      <c r="E47" s="89"/>
+      <c r="E47" s="105"/>
       <c r="F47" s="10"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3792,20 +3804,20 @@
       </c>
     </row>
     <row r="50" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="85" t="s">
+      <c r="A50" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="85"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
-      <c r="I50" s="85"/>
-      <c r="J50" s="85"/>
-      <c r="K50" s="85"/>
-      <c r="L50" s="85"/>
+      <c r="B50" s="83"/>
+      <c r="C50" s="83"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="83"/>
+      <c r="I50" s="83"/>
+      <c r="J50" s="83"/>
+      <c r="K50" s="83"/>
+      <c r="L50" s="83"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
@@ -3819,38 +3831,38 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="101" t="s">
         <v>144</v>
       </c>
-      <c r="B52" s="81"/>
-      <c r="C52" s="78" t="s">
+      <c r="B52" s="101"/>
+      <c r="C52" s="98" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="78"/>
-      <c r="E52" s="78" t="s">
+      <c r="D52" s="98"/>
+      <c r="E52" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="78"/>
-      <c r="G52" s="81" t="s">
+      <c r="F52" s="98"/>
+      <c r="G52" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="H52" s="78"/>
+      <c r="H52" s="98"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="82">
+      <c r="A53" s="111">
         <f>SUM(D47*0.5)</f>
         <v>50</v>
       </c>
-      <c r="B53" s="82"/>
-      <c r="C53" s="83"/>
-      <c r="D53" s="83"/>
-      <c r="E53" s="83"/>
-      <c r="F53" s="83"/>
-      <c r="G53" s="84">
+      <c r="B53" s="111"/>
+      <c r="C53" s="104"/>
+      <c r="D53" s="104"/>
+      <c r="E53" s="104"/>
+      <c r="F53" s="104"/>
+      <c r="G53" s="71">
         <f>SUM(C53*E53)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="84"/>
+      <c r="H53" s="71"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
@@ -3868,61 +3880,61 @@
       <c r="C56" s="10"/>
     </row>
     <row r="57" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="86" t="s">
+      <c r="A57" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="86"/>
-      <c r="C57" s="86"/>
-      <c r="D57" s="94" t="s">
+      <c r="B57" s="73"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="E57" s="94"/>
+      <c r="E57" s="96"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="88" t="s">
+      <c r="A58" s="97" t="s">
         <v>134</v>
       </c>
-      <c r="B58" s="88"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="74">
+      <c r="B58" s="97"/>
+      <c r="C58" s="97"/>
+      <c r="D58" s="95">
         <f>IF(C53="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G53)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G53)))</f>
         <v>12</v>
       </c>
-      <c r="E58" s="74"/>
+      <c r="E58" s="95"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="88" t="s">
+      <c r="A59" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="B59" s="88"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="74" t="str">
+      <c r="B59" s="97"/>
+      <c r="C59" s="97"/>
+      <c r="D59" s="95" t="str">
         <f>IFERROR((IF(SUM(12-D58)=0,"-",SUM(12-D58))),"")</f>
         <v>-</v>
       </c>
-      <c r="E59" s="74"/>
+      <c r="E59" s="95"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="84" t="s">
+      <c r="A60" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="84"/>
-      <c r="C60" s="84"/>
-      <c r="D60" s="73">
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="103">
         <v>37.5</v>
       </c>
-      <c r="E60" s="73"/>
+      <c r="E60" s="103"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="84" t="s">
+      <c r="A61" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="B61" s="84"/>
-      <c r="C61" s="84"/>
-      <c r="D61" s="73">
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="103">
         <v>25.5</v>
       </c>
-      <c r="E61" s="73"/>
+      <c r="E61" s="103"/>
       <c r="F61" s="12" t="s">
         <v>142</v>
       </c>
@@ -3938,82 +3950,175 @@
       <c r="C63" s="21"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="91" t="s">
+      <c r="A64" s="74" t="s">
         <v>272</v>
       </c>
-      <c r="B64" s="92"/>
-      <c r="C64" s="96" t="s">
+      <c r="B64" s="75"/>
+      <c r="C64" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="D64" s="84"/>
+      <c r="D64" s="71"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="92" t="s">
+      <c r="A65" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="92"/>
-      <c r="C65" s="84"/>
-      <c r="D65" s="84"/>
+      <c r="B65" s="75"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="92" t="s">
+      <c r="A66" s="75" t="s">
         <v>261</v>
       </c>
-      <c r="B66" s="92"/>
-      <c r="C66" s="84"/>
-      <c r="D66" s="84"/>
+      <c r="B66" s="75"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="71"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="92" t="s">
+      <c r="A67" s="75" t="s">
         <v>302</v>
       </c>
-      <c r="B67" s="92"/>
-      <c r="C67" s="79" t="str">
+      <c r="B67" s="75"/>
+      <c r="C67" s="92" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D67" s="79"/>
+      <c r="D67" s="92"/>
       <c r="E67" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="92" t="s">
+      <c r="A68" s="75" t="s">
         <v>262</v>
       </c>
-      <c r="B68" s="92"/>
-      <c r="C68" s="84" t="s">
+      <c r="B68" s="75"/>
+      <c r="C68" s="71" t="s">
         <v>263</v>
       </c>
-      <c r="D68" s="84"/>
+      <c r="D68" s="71"/>
       <c r="E68" s="11" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="92" t="s">
+      <c r="A69" s="75" t="s">
         <v>152</v>
       </c>
-      <c r="B69" s="92"/>
-      <c r="C69" s="84"/>
-      <c r="D69" s="84"/>
+      <c r="B69" s="75"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="71"/>
       <c r="E69" s="11" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="92" t="s">
+      <c r="A70" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="B70" s="92"/>
-      <c r="C70" s="84"/>
-      <c r="D70" s="84"/>
+      <c r="B70" s="75"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="71"/>
       <c r="E70" s="11" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="117">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J5:K6"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="I29:J29"/>
@@ -4038,99 +4143,6 @@
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="I21:J21"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="I41:J41"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C4 C7:C8 C11:C12 B37:C37 C53:E53 C64:C66 C68:C70">
     <cfRule type="expression" dxfId="8" priority="5">
@@ -4197,7 +4209,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." xr:uid="{8C7E2C1B-80DC-4BB6-92F9-B434AEC4D204}">
           <x14:formula1>
-            <xm:f>reference!$E$11:$E$14</xm:f>
+            <xm:f>reference!$J$3:$J$5</xm:f>
           </x14:formula1>
           <xm:sqref>C7:F7</xm:sqref>
         </x14:dataValidation>
@@ -7589,7 +7601,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7692,7 +7704,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7736,6 +7748,9 @@
       <c r="H2" s="65" t="s">
         <v>269</v>
       </c>
+      <c r="J2" s="65" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -7756,6 +7771,9 @@
       <c r="H3" s="66" t="s">
         <v>357</v>
       </c>
+      <c r="J3" s="66" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -7777,6 +7795,9 @@
       <c r="H4" s="66" t="s">
         <v>359</v>
       </c>
+      <c r="J4" s="66" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -7794,6 +7815,9 @@
       </c>
       <c r="H5" s="66" t="s">
         <v>361</v>
+      </c>
+      <c r="J5" s="66" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>